<commit_message>
[Silverfox] PC 발주 FMS 복구
</commit_message>
<xml_diff>
--- a/DesignDocs/Design/발주 문서/PC 발주 문서.xlsx
+++ b/DesignDocs/Design/발주 문서/PC 발주 문서.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="19126"/>
+  <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\joo sanghyen\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Silverfox_x\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{47C94662-7573-417E-B57E-2E8F99990450}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="7470" windowHeight="1545"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="7470" windowHeight="1545" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="PC" sheetId="8" r:id="rId1"/>
@@ -25,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="93" uniqueCount="90">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="91" uniqueCount="88">
   <si>
     <t>순번</t>
   </si>
@@ -101,6 +102,10 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
+    <t>Dameged_01</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
     <t>Idle_BT</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -149,10 +154,22 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
+    <t>Range_Attack_01</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
     <t>Melee_Skill_01</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
+    <t>위에서 아래로 한손으로 내리치는 모션</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Melee_Skill_02</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
     <t>아래에서 위로 올려치는 모션</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -162,6 +179,10 @@
   </si>
   <si>
     <t>슬라브 스쿼트 자세</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Range_Skill_01</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
@@ -355,39 +376,11 @@
     <t>주먹을 앞으로 하고 공격태세를 유지한다.</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
-  <si>
-    <t>Idle_02_loop</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Idle_02에서 이어지는 루프모션. 담배를 입에 문 상태로 Idle_01.</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Damaged_01</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Melee_Skill_02</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>위에서 아래로 한손으로 내리치는 모션 (가라테 챱)</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Range_01</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Range_02</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -450,7 +443,7 @@
       <charset val="129"/>
     </font>
   </fonts>
-  <fills count="8">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -469,30 +462,6 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="1" tint="0.499984740745262"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="0" tint="-0.499984740745262"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.59999389629810485"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.59999389629810485"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
   </fills>
   <borders count="12">
     <border>
@@ -666,7 +635,7 @@
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="61">
+  <cellXfs count="38">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -694,70 +663,37 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="2" fillId="6" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="6" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -784,9 +720,6 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -811,49 +744,16 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="6" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="6" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="2" fillId="6" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="2" fillId="6" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="2" fillId="5" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="표준" xfId="0" builtinId="0"/>
-    <cellStyle name="표준 2" xfId="1"/>
+    <cellStyle name="표준 2" xfId="1" xr:uid="{00000000-0005-0000-0000-000001000000}"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -888,7 +788,7 @@
         <xdr:cNvPr id="5" name="그룹 4">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00B3ABD8-A016-4750-9BDE-AB6050E1AA7D}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00B3ABD8-A016-4750-9BDE-AB6050E1AA7D}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -907,7 +807,7 @@
           <xdr:cNvPr id="6" name="그림 5">
             <a:extLst>
               <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{05A3C50E-A074-493D-82DB-B5F4F0C12322}"/>
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{05A3C50E-A074-493D-82DB-B5F4F0C12322}"/>
               </a:ext>
             </a:extLst>
           </xdr:cNvPr>
@@ -951,7 +851,7 @@
           <xdr:cNvPr id="7" name="그림 6">
             <a:extLst>
               <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{679B68F0-C347-4392-9D61-9252FE82E2F0}"/>
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{679B68F0-C347-4392-9D61-9252FE82E2F0}"/>
               </a:ext>
             </a:extLst>
           </xdr:cNvPr>
@@ -1003,6 +903,191 @@
           <a:xfrm rot="310041">
             <a:off x="7020455" y="1700739"/>
             <a:ext cx="594960" cy="523874"/>
+          </a:xfrm>
+          <a:prstGeom prst="rect">
+            <a:avLst/>
+          </a:prstGeom>
+        </xdr:spPr>
+      </xdr:pic>
+    </xdr:grpSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>23</xdr:col>
+      <xdr:colOff>189481</xdr:colOff>
+      <xdr:row>62</xdr:row>
+      <xdr:rowOff>151600</xdr:rowOff>
+    </xdr:to>
+    <xdr:grpSp>
+      <xdr:nvGrpSpPr>
+        <xdr:cNvPr id="8" name="그룹 7">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{4C3A5EE2-0C35-4B0B-A31F-7F413BAA3B12}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGrpSpPr/>
+      </xdr:nvGrpSpPr>
+      <xdr:grpSpPr>
+        <a:xfrm>
+          <a:off x="0" y="0"/>
+          <a:ext cx="15962881" cy="13143700"/>
+          <a:chOff x="0" y="0"/>
+          <a:chExt cx="15962881" cy="13143700"/>
+        </a:xfrm>
+      </xdr:grpSpPr>
+      <xdr:pic>
+        <xdr:nvPicPr>
+          <xdr:cNvPr id="2" name="그림 1">
+            <a:extLst>
+              <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{6E7792C7-909C-4652-B060-33440B7409CE}"/>
+              </a:ext>
+            </a:extLst>
+          </xdr:cNvPr>
+          <xdr:cNvPicPr>
+            <a:picLocks noChangeAspect="1"/>
+          </xdr:cNvPicPr>
+        </xdr:nvPicPr>
+        <xdr:blipFill>
+          <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+          <a:stretch>
+            <a:fillRect/>
+          </a:stretch>
+        </xdr:blipFill>
+        <xdr:spPr>
+          <a:xfrm>
+            <a:off x="0" y="0"/>
+            <a:ext cx="7876190" cy="7266667"/>
+          </a:xfrm>
+          <a:prstGeom prst="rect">
+            <a:avLst/>
+          </a:prstGeom>
+        </xdr:spPr>
+      </xdr:pic>
+      <xdr:pic>
+        <xdr:nvPicPr>
+          <xdr:cNvPr id="3" name="그림 2">
+            <a:extLst>
+              <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{9486F3DC-56DE-4D8E-9829-D490DDCD9126}"/>
+              </a:ext>
+            </a:extLst>
+          </xdr:cNvPr>
+          <xdr:cNvPicPr>
+            <a:picLocks noChangeAspect="1"/>
+          </xdr:cNvPicPr>
+        </xdr:nvPicPr>
+        <xdr:blipFill>
+          <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2"/>
+          <a:stretch>
+            <a:fillRect/>
+          </a:stretch>
+        </xdr:blipFill>
+        <xdr:spPr>
+          <a:xfrm>
+            <a:off x="7810500" y="238125"/>
+            <a:ext cx="8152381" cy="7085714"/>
+          </a:xfrm>
+          <a:prstGeom prst="rect">
+            <a:avLst/>
+          </a:prstGeom>
+        </xdr:spPr>
+      </xdr:pic>
+      <xdr:pic>
+        <xdr:nvPicPr>
+          <xdr:cNvPr id="4" name="그림 3">
+            <a:extLst>
+              <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{69AAB0F8-BE94-4300-84A3-3846722B16A0}"/>
+              </a:ext>
+            </a:extLst>
+          </xdr:cNvPr>
+          <xdr:cNvPicPr>
+            <a:picLocks noChangeAspect="1"/>
+          </xdr:cNvPicPr>
+        </xdr:nvPicPr>
+        <xdr:blipFill>
+          <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId3"/>
+          <a:stretch>
+            <a:fillRect/>
+          </a:stretch>
+        </xdr:blipFill>
+        <xdr:spPr>
+          <a:xfrm>
+            <a:off x="6743700" y="6743700"/>
+            <a:ext cx="8800000" cy="6400000"/>
+          </a:xfrm>
+          <a:prstGeom prst="rect">
+            <a:avLst/>
+          </a:prstGeom>
+        </xdr:spPr>
+      </xdr:pic>
+      <xdr:pic>
+        <xdr:nvPicPr>
+          <xdr:cNvPr id="6" name="그림 5">
+            <a:extLst>
+              <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{4A5D7FE0-F455-43DC-B6AA-980EAFD7E3DA}"/>
+              </a:ext>
+            </a:extLst>
+          </xdr:cNvPr>
+          <xdr:cNvPicPr>
+            <a:picLocks noChangeAspect="1"/>
+          </xdr:cNvPicPr>
+        </xdr:nvPicPr>
+        <xdr:blipFill>
+          <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId4"/>
+          <a:stretch>
+            <a:fillRect/>
+          </a:stretch>
+        </xdr:blipFill>
+        <xdr:spPr>
+          <a:xfrm>
+            <a:off x="190500" y="6438900"/>
+            <a:ext cx="6180952" cy="6695238"/>
+          </a:xfrm>
+          <a:prstGeom prst="rect">
+            <a:avLst/>
+          </a:prstGeom>
+        </xdr:spPr>
+      </xdr:pic>
+      <xdr:pic>
+        <xdr:nvPicPr>
+          <xdr:cNvPr id="7" name="그림 6">
+            <a:extLst>
+              <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C9CFB809-00E3-4889-BD59-3ED071DA479F}"/>
+              </a:ext>
+            </a:extLst>
+          </xdr:cNvPr>
+          <xdr:cNvPicPr>
+            <a:picLocks noChangeAspect="1"/>
+          </xdr:cNvPicPr>
+        </xdr:nvPicPr>
+        <xdr:blipFill>
+          <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId5"/>
+          <a:stretch>
+            <a:fillRect/>
+          </a:stretch>
+        </xdr:blipFill>
+        <xdr:spPr>
+          <a:xfrm>
+            <a:off x="4924425" y="6600825"/>
+            <a:ext cx="3171429" cy="6476190"/>
           </a:xfrm>
           <a:prstGeom prst="rect">
             <a:avLst/>
@@ -1311,11 +1396,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B1:G45"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
+  <dimension ref="B1:G44"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D43" sqref="D43:E43"/>
+    <sheetView topLeftCell="A19" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D33" sqref="D33:E33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12" x14ac:dyDescent="0.3"/>
@@ -1344,622 +1429,567 @@
       <c r="E2" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="F2" s="31" t="s">
+      <c r="F2" s="20" t="s">
         <v>3</v>
       </c>
-      <c r="G2" s="33" t="s">
-        <v>40</v>
+      <c r="G2" s="22" t="s">
+        <v>45</v>
       </c>
     </row>
     <row r="3" spans="2:7" ht="12" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B3" s="5" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="C3" s="7" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="D3" s="7" t="s">
-        <v>24</v>
-      </c>
-      <c r="E3" s="35"/>
-      <c r="F3" s="32"/>
-      <c r="G3" s="34"/>
+        <v>25</v>
+      </c>
+      <c r="E3" s="24"/>
+      <c r="F3" s="21"/>
+      <c r="G3" s="23"/>
     </row>
     <row r="4" spans="2:7" ht="12" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B4" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="C4" s="36" t="s">
-        <v>25</v>
-      </c>
-      <c r="D4" s="36"/>
-      <c r="E4" s="35"/>
-      <c r="F4" s="32"/>
-      <c r="G4" s="34"/>
+      <c r="C4" s="25" t="s">
+        <v>26</v>
+      </c>
+      <c r="D4" s="25"/>
+      <c r="E4" s="24"/>
+      <c r="F4" s="21"/>
+      <c r="G4" s="23"/>
     </row>
     <row r="5" spans="2:7" ht="12" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B5" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="C5" s="36" t="s">
-        <v>26</v>
-      </c>
-      <c r="D5" s="36"/>
-      <c r="E5" s="35"/>
-      <c r="F5" s="32"/>
-      <c r="G5" s="34"/>
+      <c r="C5" s="25" t="s">
+        <v>27</v>
+      </c>
+      <c r="D5" s="25"/>
+      <c r="E5" s="24"/>
+      <c r="F5" s="21"/>
+      <c r="G5" s="23"/>
     </row>
     <row r="6" spans="2:7" ht="12" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B6" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="C6" s="37" t="s">
-        <v>30</v>
-      </c>
-      <c r="D6" s="36"/>
-      <c r="E6" s="35"/>
-      <c r="F6" s="32"/>
-      <c r="G6" s="34"/>
+      <c r="C6" s="26" t="s">
+        <v>31</v>
+      </c>
+      <c r="D6" s="25"/>
+      <c r="E6" s="24"/>
+      <c r="F6" s="21"/>
+      <c r="G6" s="23"/>
     </row>
     <row r="7" spans="2:7" ht="12" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B7" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="C7" s="38" t="s">
-        <v>24</v>
-      </c>
-      <c r="D7" s="39"/>
-      <c r="E7" s="35"/>
-      <c r="F7" s="32"/>
-      <c r="G7" s="34"/>
+      <c r="C7" s="27" t="s">
+        <v>25</v>
+      </c>
+      <c r="D7" s="19"/>
+      <c r="E7" s="24"/>
+      <c r="F7" s="21"/>
+      <c r="G7" s="23"/>
     </row>
     <row r="8" spans="2:7" ht="12" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B8" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="C8" s="39" t="s">
+      <c r="C8" s="19" t="s">
         <v>19</v>
       </c>
-      <c r="D8" s="39"/>
-      <c r="E8" s="35"/>
-      <c r="F8" s="32"/>
-      <c r="G8" s="34"/>
+      <c r="D8" s="19"/>
+      <c r="E8" s="24"/>
+      <c r="F8" s="21"/>
+      <c r="G8" s="23"/>
     </row>
     <row r="9" spans="2:7" ht="12" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B9" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="C9" s="39" t="s">
-        <v>27</v>
-      </c>
-      <c r="D9" s="39"/>
-      <c r="E9" s="35"/>
-      <c r="F9" s="32"/>
-      <c r="G9" s="34"/>
+      <c r="C9" s="19" t="s">
+        <v>28</v>
+      </c>
+      <c r="D9" s="19"/>
+      <c r="E9" s="24"/>
+      <c r="F9" s="21"/>
+      <c r="G9" s="23"/>
     </row>
     <row r="10" spans="2:7" ht="12" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B10" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="C10" s="39" t="s">
-        <v>28</v>
-      </c>
-      <c r="D10" s="39"/>
-      <c r="E10" s="35"/>
-      <c r="F10" s="32"/>
-      <c r="G10" s="34"/>
+      <c r="C10" s="19" t="s">
+        <v>29</v>
+      </c>
+      <c r="D10" s="19"/>
+      <c r="E10" s="24"/>
+      <c r="F10" s="21"/>
+      <c r="G10" s="23"/>
     </row>
     <row r="11" spans="2:7" ht="12" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B11" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="C11" s="36" t="s">
-        <v>29</v>
-      </c>
-      <c r="D11" s="36"/>
-      <c r="E11" s="35"/>
-      <c r="F11" s="32"/>
-      <c r="G11" s="34"/>
+      <c r="C11" s="25" t="s">
+        <v>30</v>
+      </c>
+      <c r="D11" s="25"/>
+      <c r="E11" s="24"/>
+      <c r="F11" s="21"/>
+      <c r="G11" s="23"/>
     </row>
     <row r="12" spans="2:7" ht="228" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B12" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="C12" s="40"/>
-      <c r="D12" s="40"/>
-      <c r="E12" s="35"/>
-      <c r="F12" s="32" t="s">
+      <c r="C12" s="28"/>
+      <c r="D12" s="28"/>
+      <c r="E12" s="24"/>
+      <c r="F12" s="21" t="s">
         <v>12</v>
       </c>
-      <c r="G12" s="34"/>
+      <c r="G12" s="23"/>
     </row>
     <row r="13" spans="2:7" ht="12" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B13" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="C13" s="42"/>
-      <c r="D13" s="42"/>
-      <c r="E13" s="35"/>
-      <c r="F13" s="32"/>
-      <c r="G13" s="41"/>
+      <c r="C13" s="30"/>
+      <c r="D13" s="30"/>
+      <c r="E13" s="24"/>
+      <c r="F13" s="21"/>
+      <c r="G13" s="29"/>
     </row>
     <row r="14" spans="2:7" ht="12" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B14" s="43" t="s">
+      <c r="B14" s="31" t="s">
         <v>14</v>
       </c>
-      <c r="C14" s="44"/>
-      <c r="D14" s="45" t="s">
+      <c r="C14" s="32"/>
+      <c r="D14" s="33" t="s">
         <v>15</v>
       </c>
-      <c r="E14" s="44"/>
-      <c r="F14" s="46" t="s">
+      <c r="E14" s="32"/>
+      <c r="F14" s="34" t="s">
         <v>16</v>
       </c>
-      <c r="G14" s="47"/>
+      <c r="G14" s="35"/>
     </row>
     <row r="15" spans="2:7" ht="12" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B15" s="29" t="s">
+      <c r="B15" s="18" t="s">
         <v>20</v>
       </c>
-      <c r="C15" s="30"/>
-      <c r="D15" s="11" t="s">
-        <v>55</v>
+      <c r="C15" s="19"/>
+      <c r="D15" s="16" t="s">
+        <v>60</v>
       </c>
       <c r="E15" s="10"/>
-      <c r="F15" s="12">
-        <v>43220</v>
-      </c>
-      <c r="G15" s="13"/>
+      <c r="F15" s="13"/>
+      <c r="G15" s="14"/>
     </row>
     <row r="16" spans="2:7" ht="12" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B16" s="29" t="s">
-        <v>31</v>
-      </c>
-      <c r="C16" s="30"/>
-      <c r="D16" s="11" t="s">
-        <v>56</v>
+      <c r="B16" s="18" t="s">
+        <v>32</v>
+      </c>
+      <c r="C16" s="19"/>
+      <c r="D16" s="16" t="s">
+        <v>61</v>
       </c>
       <c r="E16" s="10"/>
-      <c r="F16" s="12">
-        <v>43220</v>
-      </c>
-      <c r="G16" s="13"/>
+      <c r="F16" s="13"/>
+      <c r="G16" s="14"/>
     </row>
     <row r="17" spans="2:7" ht="12" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B17" s="50" t="s">
-        <v>83</v>
-      </c>
-      <c r="C17" s="51"/>
-      <c r="D17" s="11" t="s">
-        <v>84</v>
+      <c r="B17" s="18" t="s">
+        <v>23</v>
+      </c>
+      <c r="C17" s="19"/>
+      <c r="D17" s="16" t="s">
+        <v>87</v>
       </c>
       <c r="E17" s="10"/>
-      <c r="F17" s="52">
-        <v>43220</v>
-      </c>
-      <c r="G17" s="53"/>
+      <c r="F17" s="13"/>
+      <c r="G17" s="14"/>
     </row>
     <row r="18" spans="2:7" ht="12" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B18" s="29" t="s">
-        <v>22</v>
-      </c>
-      <c r="C18" s="30"/>
-      <c r="D18" s="11" t="s">
-        <v>82</v>
+      <c r="B18" s="36" t="s">
+        <v>17</v>
+      </c>
+      <c r="C18" s="13"/>
+      <c r="D18" s="16" t="s">
+        <v>62</v>
       </c>
       <c r="E18" s="10"/>
-      <c r="F18" s="12">
-        <v>43222</v>
-      </c>
-      <c r="G18" s="13"/>
+      <c r="F18" s="13"/>
+      <c r="G18" s="14"/>
     </row>
     <row r="19" spans="2:7" ht="12" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B19" s="48" t="s">
-        <v>17</v>
-      </c>
-      <c r="C19" s="49"/>
-      <c r="D19" s="11" t="s">
-        <v>57</v>
+      <c r="B19" s="9" t="s">
+        <v>21</v>
+      </c>
+      <c r="C19" s="10"/>
+      <c r="D19" s="16" t="s">
+        <v>51</v>
       </c>
       <c r="E19" s="10"/>
-      <c r="F19" s="12">
-        <v>43222</v>
-      </c>
-      <c r="G19" s="13"/>
+      <c r="F19" s="13"/>
+      <c r="G19" s="14"/>
     </row>
     <row r="20" spans="2:7" ht="12" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B20" s="9" t="s">
-        <v>21</v>
+        <v>33</v>
       </c>
       <c r="C20" s="10"/>
-      <c r="D20" s="11" t="s">
-        <v>46</v>
+      <c r="D20" s="16" t="s">
+        <v>52</v>
       </c>
       <c r="E20" s="10"/>
-      <c r="F20" s="12">
-        <v>43223</v>
-      </c>
-      <c r="G20" s="13"/>
+      <c r="F20" s="13"/>
+      <c r="G20" s="14"/>
     </row>
     <row r="21" spans="2:7" ht="12" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B21" s="9" t="s">
-        <v>32</v>
+        <v>22</v>
       </c>
       <c r="C21" s="10"/>
-      <c r="D21" s="11" t="s">
-        <v>47</v>
+      <c r="D21" s="16" t="s">
+        <v>63</v>
       </c>
       <c r="E21" s="10"/>
-      <c r="F21" s="12">
-        <v>43223</v>
-      </c>
-      <c r="G21" s="13"/>
+      <c r="F21" s="16"/>
+      <c r="G21" s="17"/>
     </row>
     <row r="22" spans="2:7" ht="12" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B22" s="9" t="s">
-        <v>85</v>
+        <v>73</v>
       </c>
       <c r="C22" s="10"/>
       <c r="D22" s="11" t="s">
-        <v>58</v>
-      </c>
-      <c r="E22" s="10"/>
-      <c r="F22" s="52">
-        <v>43228</v>
-      </c>
-      <c r="G22" s="54"/>
+        <v>74</v>
+      </c>
+      <c r="E22" s="12"/>
+      <c r="F22" s="13"/>
+      <c r="G22" s="14"/>
     </row>
     <row r="23" spans="2:7" ht="12" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B23" s="9" t="s">
-        <v>68</v>
+        <v>34</v>
       </c>
       <c r="C23" s="10"/>
       <c r="D23" s="11" t="s">
-        <v>69</v>
-      </c>
-      <c r="E23" s="10"/>
-      <c r="F23" s="12">
-        <v>43228</v>
-      </c>
-      <c r="G23" s="13"/>
+        <v>48</v>
+      </c>
+      <c r="E23" s="12"/>
+      <c r="F23" s="13"/>
+      <c r="G23" s="14"/>
     </row>
     <row r="24" spans="2:7" ht="12" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B24" s="9" t="s">
-        <v>33</v>
+        <v>46</v>
       </c>
       <c r="C24" s="10"/>
       <c r="D24" s="11" t="s">
-        <v>43</v>
-      </c>
-      <c r="E24" s="10"/>
-      <c r="F24" s="12">
-        <v>43229</v>
-      </c>
-      <c r="G24" s="13"/>
+        <v>49</v>
+      </c>
+      <c r="E24" s="12"/>
+      <c r="F24" s="13"/>
+      <c r="G24" s="14"/>
     </row>
     <row r="25" spans="2:7" ht="12" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B25" s="9" t="s">
-        <v>41</v>
+        <v>47</v>
       </c>
       <c r="C25" s="10"/>
       <c r="D25" s="11" t="s">
-        <v>44</v>
-      </c>
-      <c r="E25" s="10"/>
-      <c r="F25" s="12">
-        <v>43229</v>
-      </c>
-      <c r="G25" s="13"/>
+        <v>50</v>
+      </c>
+      <c r="E25" s="12"/>
+      <c r="F25" s="13"/>
+      <c r="G25" s="14"/>
     </row>
     <row r="26" spans="2:7" ht="32.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B26" s="9" t="s">
-        <v>42</v>
+        <v>35</v>
       </c>
       <c r="C26" s="10"/>
-      <c r="D26" s="11" t="s">
-        <v>45</v>
-      </c>
-      <c r="E26" s="10"/>
-      <c r="F26" s="12">
-        <v>43229</v>
-      </c>
-      <c r="G26" s="13"/>
+      <c r="D26" s="15" t="s">
+        <v>57</v>
+      </c>
+      <c r="E26" s="12"/>
+      <c r="F26" s="16"/>
+      <c r="G26" s="17"/>
     </row>
     <row r="27" spans="2:7" ht="32.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B27" s="9" t="s">
-        <v>88</v>
+        <v>43</v>
       </c>
       <c r="C27" s="10"/>
-      <c r="D27" s="56" t="s">
-        <v>52</v>
-      </c>
-      <c r="E27" s="10"/>
-      <c r="F27" s="52">
-        <v>43230</v>
-      </c>
-      <c r="G27" s="54"/>
+      <c r="D27" s="15" t="s">
+        <v>58</v>
+      </c>
+      <c r="E27" s="12"/>
+      <c r="F27" s="16"/>
+      <c r="G27" s="17"/>
     </row>
     <row r="28" spans="2:7" ht="32.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B28" s="28" t="s">
-        <v>38</v>
-      </c>
-      <c r="C28" s="26"/>
-      <c r="D28" s="25" t="s">
-        <v>53</v>
-      </c>
-      <c r="E28" s="26"/>
-      <c r="F28" s="55"/>
-      <c r="G28" s="57"/>
+      <c r="B28" s="9" t="s">
+        <v>44</v>
+      </c>
+      <c r="C28" s="10"/>
+      <c r="D28" s="15" t="s">
+        <v>59</v>
+      </c>
+      <c r="E28" s="12"/>
+      <c r="F28" s="16"/>
+      <c r="G28" s="17"/>
     </row>
     <row r="29" spans="2:7" ht="12" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B29" s="28" t="s">
-        <v>39</v>
-      </c>
-      <c r="C29" s="26"/>
-      <c r="D29" s="25" t="s">
-        <v>54</v>
-      </c>
-      <c r="E29" s="26"/>
-      <c r="F29" s="55"/>
-      <c r="G29" s="57"/>
+      <c r="B29" s="9" t="s">
+        <v>36</v>
+      </c>
+      <c r="C29" s="10"/>
+      <c r="D29" s="11" t="s">
+        <v>37</v>
+      </c>
+      <c r="E29" s="12"/>
+      <c r="F29" s="16"/>
+      <c r="G29" s="17"/>
     </row>
     <row r="30" spans="2:7" ht="12" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B30" s="9" t="s">
-        <v>34</v>
+        <v>38</v>
       </c>
       <c r="C30" s="10"/>
       <c r="D30" s="11" t="s">
-        <v>87</v>
-      </c>
-      <c r="E30" s="10"/>
-      <c r="F30" s="52">
-        <v>43235</v>
-      </c>
-      <c r="G30" s="54"/>
+        <v>39</v>
+      </c>
+      <c r="E30" s="12"/>
+      <c r="F30" s="16"/>
+      <c r="G30" s="17"/>
     </row>
     <row r="31" spans="2:7" ht="29.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B31" s="18" t="s">
-        <v>86</v>
-      </c>
-      <c r="C31" s="15"/>
-      <c r="D31" s="19" t="s">
-        <v>35</v>
-      </c>
-      <c r="E31" s="15"/>
-      <c r="F31" s="19"/>
-      <c r="G31" s="60"/>
+      <c r="B31" s="9" t="s">
+        <v>42</v>
+      </c>
+      <c r="C31" s="10"/>
+      <c r="D31" s="15" t="s">
+        <v>64</v>
+      </c>
+      <c r="E31" s="12"/>
+      <c r="F31" s="16"/>
+      <c r="G31" s="17"/>
     </row>
     <row r="32" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B32" s="9" t="s">
-        <v>89</v>
-      </c>
-      <c r="C32" s="10"/>
-      <c r="D32" s="56" t="s">
-        <v>59</v>
+      <c r="B32" s="36" t="s">
+        <v>53</v>
+      </c>
+      <c r="C32" s="13"/>
+      <c r="D32" s="16" t="s">
+        <v>55</v>
       </c>
       <c r="E32" s="10"/>
-      <c r="F32" s="52">
-        <v>43236</v>
-      </c>
-      <c r="G32" s="54"/>
+      <c r="F32" s="13"/>
+      <c r="G32" s="14"/>
     </row>
     <row r="33" spans="2:7" ht="40.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B33" s="23" t="s">
-        <v>48</v>
-      </c>
-      <c r="C33" s="24"/>
-      <c r="D33" s="55" t="s">
-        <v>50</v>
-      </c>
-      <c r="E33" s="26"/>
-      <c r="F33" s="24"/>
-      <c r="G33" s="27"/>
+      <c r="B33" s="36" t="s">
+        <v>54</v>
+      </c>
+      <c r="C33" s="13"/>
+      <c r="D33" s="37" t="s">
+        <v>56</v>
+      </c>
+      <c r="E33" s="10"/>
+      <c r="F33" s="13"/>
+      <c r="G33" s="14"/>
     </row>
     <row r="34" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B34" s="23" t="s">
-        <v>49</v>
-      </c>
-      <c r="C34" s="24"/>
-      <c r="D34" s="25" t="s">
-        <v>51</v>
-      </c>
-      <c r="E34" s="26"/>
-      <c r="F34" s="24"/>
-      <c r="G34" s="27"/>
+      <c r="B34" s="9" t="s">
+        <v>65</v>
+      </c>
+      <c r="C34" s="10"/>
+      <c r="D34" s="16" t="s">
+        <v>66</v>
+      </c>
+      <c r="E34" s="10"/>
+      <c r="F34" s="16"/>
+      <c r="G34" s="17"/>
     </row>
     <row r="35" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B35" s="18" t="s">
-        <v>60</v>
-      </c>
-      <c r="C35" s="15"/>
-      <c r="D35" s="19" t="s">
-        <v>61</v>
-      </c>
-      <c r="E35" s="15"/>
-      <c r="F35" s="19"/>
-      <c r="G35" s="60"/>
+      <c r="B35" s="9" t="s">
+        <v>67</v>
+      </c>
+      <c r="C35" s="10"/>
+      <c r="D35" s="16" t="s">
+        <v>70</v>
+      </c>
+      <c r="E35" s="10"/>
+      <c r="F35" s="16"/>
+      <c r="G35" s="17"/>
     </row>
     <row r="36" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B36" s="59" t="s">
-        <v>62</v>
-      </c>
-      <c r="C36" s="21"/>
-      <c r="D36" s="20" t="s">
-        <v>65</v>
-      </c>
-      <c r="E36" s="21"/>
-      <c r="F36" s="20"/>
-      <c r="G36" s="22"/>
+      <c r="B36" s="9" t="s">
+        <v>69</v>
+      </c>
+      <c r="C36" s="10"/>
+      <c r="D36" s="16" t="s">
+        <v>71</v>
+      </c>
+      <c r="E36" s="10"/>
+      <c r="F36" s="16"/>
+      <c r="G36" s="17"/>
     </row>
     <row r="37" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B37" s="59" t="s">
-        <v>64</v>
-      </c>
-      <c r="C37" s="21"/>
-      <c r="D37" s="20" t="s">
-        <v>66</v>
-      </c>
-      <c r="E37" s="21"/>
-      <c r="F37" s="20"/>
-      <c r="G37" s="22"/>
+      <c r="B37" s="9" t="s">
+        <v>68</v>
+      </c>
+      <c r="C37" s="10"/>
+      <c r="D37" s="16" t="s">
+        <v>72</v>
+      </c>
+      <c r="E37" s="10"/>
+      <c r="F37" s="16"/>
+      <c r="G37" s="17"/>
     </row>
     <row r="38" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B38" s="59" t="s">
-        <v>63</v>
-      </c>
-      <c r="C38" s="21"/>
-      <c r="D38" s="20" t="s">
-        <v>67</v>
-      </c>
-      <c r="E38" s="21"/>
-      <c r="F38" s="20"/>
-      <c r="G38" s="22"/>
+      <c r="B38" s="9" t="s">
+        <v>40</v>
+      </c>
+      <c r="C38" s="10"/>
+      <c r="D38" s="11" t="s">
+        <v>41</v>
+      </c>
+      <c r="E38" s="12"/>
+      <c r="F38" s="13"/>
+      <c r="G38" s="14"/>
     </row>
     <row r="39" spans="2:7" ht="41.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B39" s="9" t="s">
-        <v>36</v>
+        <v>75</v>
       </c>
       <c r="C39" s="10"/>
-      <c r="D39" s="11" t="s">
-        <v>37</v>
-      </c>
-      <c r="E39" s="10"/>
-      <c r="F39" s="12">
-        <v>43224</v>
-      </c>
-      <c r="G39" s="13"/>
+      <c r="D39" s="15" t="s">
+        <v>76</v>
+      </c>
+      <c r="E39" s="12"/>
+      <c r="F39" s="13"/>
+      <c r="G39" s="14"/>
     </row>
     <row r="40" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B40" s="28" t="s">
-        <v>70</v>
-      </c>
-      <c r="C40" s="26"/>
-      <c r="D40" s="25" t="s">
-        <v>71</v>
-      </c>
-      <c r="E40" s="26"/>
-      <c r="F40" s="58">
-        <v>43224</v>
-      </c>
-      <c r="G40" s="27"/>
+      <c r="B40" s="9" t="s">
+        <v>77</v>
+      </c>
+      <c r="C40" s="10"/>
+      <c r="D40" s="11" t="s">
+        <v>78</v>
+      </c>
+      <c r="E40" s="12"/>
+      <c r="F40" s="13"/>
+      <c r="G40" s="14"/>
     </row>
     <row r="41" spans="2:7" ht="29.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B41" s="18" t="s">
-        <v>72</v>
-      </c>
-      <c r="C41" s="15"/>
-      <c r="D41" s="19" t="s">
-        <v>73</v>
-      </c>
-      <c r="E41" s="15"/>
-      <c r="F41" s="16"/>
-      <c r="G41" s="17"/>
+      <c r="B41" s="9" t="s">
+        <v>81</v>
+      </c>
+      <c r="C41" s="10"/>
+      <c r="D41" s="15" t="s">
+        <v>79</v>
+      </c>
+      <c r="E41" s="12"/>
+      <c r="F41" s="13"/>
+      <c r="G41" s="14"/>
     </row>
     <row r="42" spans="2:7" ht="33" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B42" s="18" t="s">
-        <v>76</v>
-      </c>
-      <c r="C42" s="15"/>
-      <c r="D42" s="14" t="s">
-        <v>74</v>
-      </c>
-      <c r="E42" s="15"/>
-      <c r="F42" s="16"/>
-      <c r="G42" s="17"/>
+      <c r="B42" s="9" t="s">
+        <v>82</v>
+      </c>
+      <c r="C42" s="10"/>
+      <c r="D42" s="15" t="s">
+        <v>80</v>
+      </c>
+      <c r="E42" s="12"/>
+      <c r="F42" s="13"/>
+      <c r="G42" s="14"/>
     </row>
     <row r="43" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B43" s="18" t="s">
-        <v>77</v>
-      </c>
-      <c r="C43" s="15"/>
-      <c r="D43" s="14" t="s">
-        <v>75</v>
-      </c>
-      <c r="E43" s="15"/>
-      <c r="F43" s="16"/>
-      <c r="G43" s="17"/>
+      <c r="B43" s="9" t="s">
+        <v>83</v>
+      </c>
+      <c r="C43" s="10"/>
+      <c r="D43" s="11" t="s">
+        <v>84</v>
+      </c>
+      <c r="E43" s="12"/>
+      <c r="F43" s="13"/>
+      <c r="G43" s="14"/>
     </row>
     <row r="44" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B44" s="9" t="s">
-        <v>78</v>
+        <v>86</v>
       </c>
       <c r="C44" s="10"/>
       <c r="D44" s="11" t="s">
-        <v>79</v>
-      </c>
-      <c r="E44" s="10"/>
-      <c r="F44" s="12">
-        <v>43234</v>
-      </c>
-      <c r="G44" s="13"/>
-    </row>
-    <row r="45" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B45" s="9" t="s">
-        <v>81</v>
-      </c>
-      <c r="C45" s="10"/>
-      <c r="D45" s="11" t="s">
-        <v>80</v>
-      </c>
-      <c r="E45" s="10"/>
-      <c r="F45" s="12">
-        <v>43234</v>
-      </c>
-      <c r="G45" s="13"/>
+        <v>85</v>
+      </c>
+      <c r="E44" s="12"/>
+      <c r="F44" s="13"/>
+      <c r="G44" s="14"/>
     </row>
   </sheetData>
-  <mergeCells count="111">
+  <mergeCells count="108">
     <mergeCell ref="B32:C32"/>
-    <mergeCell ref="D40:E40"/>
-    <mergeCell ref="F40:G40"/>
-    <mergeCell ref="B40:C40"/>
+    <mergeCell ref="B27:C27"/>
+    <mergeCell ref="B28:C28"/>
+    <mergeCell ref="B39:C39"/>
+    <mergeCell ref="D34:E34"/>
+    <mergeCell ref="F34:G34"/>
+    <mergeCell ref="B37:C37"/>
+    <mergeCell ref="D37:E37"/>
+    <mergeCell ref="B35:C35"/>
     <mergeCell ref="D35:E35"/>
     <mergeCell ref="F35:G35"/>
-    <mergeCell ref="B38:C38"/>
-    <mergeCell ref="D38:E38"/>
     <mergeCell ref="B36:C36"/>
-    <mergeCell ref="D36:E36"/>
-    <mergeCell ref="F36:G36"/>
-    <mergeCell ref="B37:C37"/>
-    <mergeCell ref="B22:C22"/>
-    <mergeCell ref="D22:E22"/>
-    <mergeCell ref="F22:G22"/>
-    <mergeCell ref="B24:C24"/>
-    <mergeCell ref="D24:E24"/>
-    <mergeCell ref="F24:G24"/>
-    <mergeCell ref="D33:E33"/>
-    <mergeCell ref="F33:G33"/>
-    <mergeCell ref="F27:G27"/>
+    <mergeCell ref="B41:C41"/>
+    <mergeCell ref="B21:C21"/>
+    <mergeCell ref="D21:E21"/>
+    <mergeCell ref="F21:G21"/>
+    <mergeCell ref="B23:C23"/>
+    <mergeCell ref="D23:E23"/>
+    <mergeCell ref="F23:G23"/>
+    <mergeCell ref="D32:E32"/>
+    <mergeCell ref="F32:G32"/>
+    <mergeCell ref="F26:G26"/>
+    <mergeCell ref="F29:G29"/>
     <mergeCell ref="F30:G30"/>
     <mergeCell ref="F31:G31"/>
-    <mergeCell ref="F32:G32"/>
-    <mergeCell ref="D27:E27"/>
+    <mergeCell ref="D26:E26"/>
+    <mergeCell ref="D29:E29"/>
     <mergeCell ref="D30:E30"/>
     <mergeCell ref="D31:E31"/>
-    <mergeCell ref="D32:E32"/>
+    <mergeCell ref="D27:E27"/>
+    <mergeCell ref="F27:G27"/>
     <mergeCell ref="D28:E28"/>
     <mergeCell ref="F28:G28"/>
-    <mergeCell ref="D29:E29"/>
-    <mergeCell ref="F29:G29"/>
-    <mergeCell ref="B27:C27"/>
+    <mergeCell ref="B26:C26"/>
+    <mergeCell ref="B29:C29"/>
     <mergeCell ref="B30:C30"/>
     <mergeCell ref="B31:C31"/>
-    <mergeCell ref="B33:C33"/>
     <mergeCell ref="B15:C15"/>
     <mergeCell ref="D15:E15"/>
     <mergeCell ref="F15:G15"/>
     <mergeCell ref="B14:C14"/>
     <mergeCell ref="D14:E14"/>
     <mergeCell ref="F14:G14"/>
-    <mergeCell ref="B19:C19"/>
-    <mergeCell ref="D19:E19"/>
-    <mergeCell ref="F19:G19"/>
-    <mergeCell ref="B16:C16"/>
-    <mergeCell ref="D16:E16"/>
-    <mergeCell ref="F16:G16"/>
-    <mergeCell ref="B17:C17"/>
-    <mergeCell ref="D17:E17"/>
-    <mergeCell ref="F17:G17"/>
+    <mergeCell ref="B18:C18"/>
+    <mergeCell ref="D18:E18"/>
+    <mergeCell ref="F18:G18"/>
     <mergeCell ref="F2:F11"/>
     <mergeCell ref="G2:G11"/>
     <mergeCell ref="E3:E13"/>
@@ -1975,51 +2005,53 @@
     <mergeCell ref="F12:F13"/>
     <mergeCell ref="G12:G13"/>
     <mergeCell ref="C13:D13"/>
-    <mergeCell ref="B21:C21"/>
-    <mergeCell ref="D21:E21"/>
-    <mergeCell ref="F21:G21"/>
-    <mergeCell ref="B18:C18"/>
-    <mergeCell ref="D18:E18"/>
-    <mergeCell ref="F18:G18"/>
+    <mergeCell ref="B16:C16"/>
+    <mergeCell ref="D16:E16"/>
+    <mergeCell ref="F16:G16"/>
     <mergeCell ref="B20:C20"/>
     <mergeCell ref="D20:E20"/>
     <mergeCell ref="F20:G20"/>
-    <mergeCell ref="B41:C41"/>
-    <mergeCell ref="D41:E41"/>
-    <mergeCell ref="F41:G41"/>
-    <mergeCell ref="D37:E37"/>
-    <mergeCell ref="F37:G37"/>
-    <mergeCell ref="B23:C23"/>
-    <mergeCell ref="D23:E23"/>
-    <mergeCell ref="F23:G23"/>
-    <mergeCell ref="B26:C26"/>
-    <mergeCell ref="D26:E26"/>
-    <mergeCell ref="F26:G26"/>
+    <mergeCell ref="B17:C17"/>
+    <mergeCell ref="D17:E17"/>
+    <mergeCell ref="F17:G17"/>
+    <mergeCell ref="B19:C19"/>
+    <mergeCell ref="D19:E19"/>
+    <mergeCell ref="F19:G19"/>
+    <mergeCell ref="D39:E39"/>
+    <mergeCell ref="F39:G39"/>
+    <mergeCell ref="B40:C40"/>
+    <mergeCell ref="D40:E40"/>
+    <mergeCell ref="F40:G40"/>
+    <mergeCell ref="D36:E36"/>
+    <mergeCell ref="F36:G36"/>
+    <mergeCell ref="B22:C22"/>
+    <mergeCell ref="D22:E22"/>
+    <mergeCell ref="F22:G22"/>
     <mergeCell ref="B25:C25"/>
     <mergeCell ref="D25:E25"/>
     <mergeCell ref="F25:G25"/>
+    <mergeCell ref="B24:C24"/>
+    <mergeCell ref="D24:E24"/>
+    <mergeCell ref="F24:G24"/>
+    <mergeCell ref="F37:G37"/>
+    <mergeCell ref="B38:C38"/>
+    <mergeCell ref="D38:E38"/>
     <mergeCell ref="F38:G38"/>
-    <mergeCell ref="B39:C39"/>
-    <mergeCell ref="D39:E39"/>
-    <mergeCell ref="F39:G39"/>
+    <mergeCell ref="B33:C33"/>
+    <mergeCell ref="D33:E33"/>
+    <mergeCell ref="F33:G33"/>
     <mergeCell ref="B34:C34"/>
-    <mergeCell ref="D34:E34"/>
-    <mergeCell ref="F34:G34"/>
-    <mergeCell ref="B35:C35"/>
-    <mergeCell ref="B28:C28"/>
-    <mergeCell ref="B29:C29"/>
+    <mergeCell ref="B43:C43"/>
+    <mergeCell ref="D43:E43"/>
+    <mergeCell ref="F43:G43"/>
     <mergeCell ref="B44:C44"/>
     <mergeCell ref="D44:E44"/>
     <mergeCell ref="F44:G44"/>
-    <mergeCell ref="B45:C45"/>
-    <mergeCell ref="D45:E45"/>
-    <mergeCell ref="F45:G45"/>
+    <mergeCell ref="D41:E41"/>
+    <mergeCell ref="F41:G41"/>
+    <mergeCell ref="B42:C42"/>
     <mergeCell ref="D42:E42"/>
     <mergeCell ref="F42:G42"/>
-    <mergeCell ref="B43:C43"/>
-    <mergeCell ref="D43:E43"/>
-    <mergeCell ref="F43:G43"/>
-    <mergeCell ref="B42:C42"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2028,11 +2060,11 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{19150487-6023-454D-8A40-7991F9762BEE}">
   <dimension ref="A1:Q31"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F5" sqref="F5"/>
+    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
+      <selection activeCell="Y12" sqref="Y12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -2629,5 +2661,6 @@
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>